<commit_message>
More test sets added
</commit_message>
<xml_diff>
--- a/pyfeng/data/heston_benchmark.xlsx
+++ b/pyfeng/data/heston_benchmark.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PyFENG\pyfeng\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237ADAE5-ABC7-4429-B45C-C88CC4FF9CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9E0357-D9D3-49F6-AF0E-6062BE3514EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="743" xr2:uid="{CFD8C97F-677E-4081-BE35-9D7DB797B3CD}"/>
   </bookViews>
@@ -21,6 +21,9 @@
     <sheet name="5" sheetId="5" r:id="rId6"/>
     <sheet name="6" sheetId="6" r:id="rId7"/>
     <sheet name="7" sheetId="8" r:id="rId8"/>
+    <sheet name="8" sheetId="34" r:id="rId9"/>
+    <sheet name="9" sheetId="33" r:id="rId10"/>
+    <sheet name="10" sheetId="35" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
   <si>
     <t>sigma</t>
   </si>
@@ -129,6 +132,18 @@
   </si>
   <si>
     <t>Strike</t>
+  </si>
+  <si>
+    <t>CP</t>
+  </si>
+  <si>
+    <t>divr</t>
+  </si>
+  <si>
+    <t>https://financepress.com/2019/02/15/heston-model-reference-prices/</t>
+  </si>
+  <si>
+    <t>Table A3, Figure 3 (Set I) in von Sydow et al. (2018). BENCHOP - SLV. https://doi.org/10.1080/00207160.2018.1544368</t>
   </si>
 </sst>
 </file>
@@ -139,10 +154,18 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -171,10 +194,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -182,8 +206,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -496,22 +524,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0584B610-149E-4DFB-B94E-F604CBCB4976}">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="6" max="6" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.453125" customWidth="1"/>
+    <col min="8" max="8" width="4.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -540,19 +569,22 @@
         <v>10</v>
       </c>
       <c r="J1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" t="s">
         <v>19</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>20</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -581,23 +613,26 @@
       <c r="I2" s="5">
         <v>0</v>
       </c>
-      <c r="J2" s="6">
+      <c r="J2" s="5">
+        <v>0</v>
+      </c>
+      <c r="K2" s="6">
         <f>4*C2*F2/(D2*D2)</f>
         <v>0.08</v>
       </c>
-      <c r="K2" s="5">
+      <c r="L2" s="5">
         <f>2*B2*F2*EXP(-F2*G2)/(D2*D2)/(1-EXP(-F2*G2))</f>
         <v>2.7134619625216925E-4</v>
       </c>
-      <c r="L2" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="L2" ca="1">INDIRECT(A2&amp;"!$B$1")</f>
+      <c r="M2" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="M2" ca="1">INDIRECT(A2&amp;"!$B$1")</f>
         <v>Price</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <f t="shared" ref="A3:A5" si="0">A2+1</f>
         <v>2</v>
@@ -627,23 +662,26 @@
       <c r="I3" s="5">
         <v>0.05</v>
       </c>
-      <c r="J3" s="6">
-        <f t="shared" ref="J3:J8" si="1">4*C3*F3/(D3*D3)</f>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="K3" s="6">
+        <f t="shared" ref="K3:K10" si="1">4*C3*F3/(D3*D3)</f>
         <v>0.36</v>
       </c>
-      <c r="K3" s="5">
-        <f t="shared" ref="K3:K8" si="2">2*B3*F3*EXP(-F3*G3)/(D3*D3)/(1-EXP(-F3*G3))</f>
+      <c r="L3" s="5">
+        <f t="shared" ref="L3:L9" si="2">2*B3*F3*EXP(-F3*G3)/(D3*D3)/(1-EXP(-F3*G3))</f>
         <v>1.2210578831347615E-3</v>
       </c>
-      <c r="L3" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="L3" ca="1">INDIRECT(A3&amp;"!$B$1")</f>
+      <c r="M3" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="M3" ca="1">INDIRECT(A3&amp;"!$B$1")</f>
         <v>Price</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -673,23 +711,26 @@
       <c r="I4" s="5">
         <v>0</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="6">
         <f t="shared" si="1"/>
         <v>5.9259259259259255E-2</v>
       </c>
-      <c r="K4" s="5">
+      <c r="L4" s="5">
         <f t="shared" si="2"/>
         <v>3.3285311711068295E-4</v>
       </c>
-      <c r="L4" s="3" t="str" cm="1">
-        <f t="array" aca="1" ref="L4" ca="1">INDIRECT(A4&amp;"!$B$1")</f>
+      <c r="M4" s="3" t="str" cm="1">
+        <f t="array" aca="1" ref="M4" ca="1">INDIRECT(A4&amp;"!$B$1")</f>
         <v>Price</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -718,22 +759,25 @@
       <c r="I5" s="5">
         <v>3.1899999999999998E-2</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+      <c r="K5" s="6">
         <f t="shared" si="1"/>
         <v>1.268368718086536</v>
       </c>
-      <c r="K5" s="5">
+      <c r="L5" s="5">
         <f t="shared" si="2"/>
         <v>6.8550309401436851E-4</v>
       </c>
-      <c r="L5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <f t="shared" ref="A6" si="4">A5+1</f>
         <v>5</v>
@@ -762,22 +806,25 @@
       <c r="I6" s="5">
         <v>0.05</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+      <c r="K6" s="6">
         <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
-      <c r="K6" s="5">
+      <c r="L6" s="5">
         <f t="shared" si="2"/>
         <v>1.6344716763487597E-5</v>
       </c>
-      <c r="L6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -805,22 +852,25 @@
       <c r="I7" s="5">
         <v>0</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6">
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-      <c r="K7" s="5">
+      <c r="L7" s="5">
         <f t="shared" si="2"/>
         <v>3.6321592807750218E-6</v>
       </c>
-      <c r="L7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N7" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -848,24 +898,303 @@
       <c r="I8" s="5">
         <v>0</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="6">
         <f t="shared" si="1"/>
         <v>0.90353478515184005</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L8" s="5">
         <f t="shared" si="2"/>
         <v>2.3645603493803969E-3</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="M8" s="2" t="s">
+      <c r="M8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N8" s="2" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="F9" s="5">
+        <v>4</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>100</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="K9" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L9" s="5">
+        <f t="shared" si="2"/>
+        <v>5.9703553164076953E-3</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="F10" s="5">
+        <v>4</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="H10" s="5">
+        <v>100</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0.02</v>
+      </c>
+      <c r="K10" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="L10" s="5">
+        <f t="shared" ref="L10:L11" si="5">2*B10*F10*EXP(-F10*G10)/(D10*D10)/(1-EXP(-F10*G10))</f>
+        <v>1.9602666595558249</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N10" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.114</v>
+      </c>
+      <c r="C11" s="5">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>-0.36</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2.58</v>
+      </c>
+      <c r="G11" s="5">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5">
+        <v>100</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="6">
+        <f t="shared" ref="K11" si="6">4*C11*F11/(D11*D11)</f>
+        <v>0.44375999999999999</v>
+      </c>
+      <c r="L11" s="5">
+        <f t="shared" si="5"/>
+        <v>4.8227706557066388E-2</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="O11" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N9" r:id="rId1" xr:uid="{7031F408-D0C8-4303-980A-BE75B855310D}"/>
+    <hyperlink ref="N10" r:id="rId2" xr:uid="{875806D3-0B48-4136-831B-3F4391F03BDC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{437B921E-6D3A-47EC-9DF4-CC9958C57C5F}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>90</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2" s="7">
+        <v>4.5183603586861701E-8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>95</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <v>4.6195485565385098E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>0.47778117162950401</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>105</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2.5274478231946999E-6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>110</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1.2993276005262401E-13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAE028F6-A224-4AC3-A0F7-14C744EB35E2}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <f>100*(100/75)</f>
+        <v>133.33333333333331</v>
+      </c>
+      <c r="B2" s="1">
+        <f>0.908502728459621*(100/75)</f>
+        <v>1.2113369712794946</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3" s="1">
+        <f>9.04665011922096</f>
+        <v>9.0466501192209599</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f>100*(100/125)</f>
+        <v>80</v>
+      </c>
+      <c r="B4" s="1">
+        <f>28.5147863992987*(100/125)</f>
+        <v>22.811829119438961</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -873,7 +1202,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5761A8C7-5DBE-4514-94EE-A5933B58C928}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -929,7 +1260,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FCD568-C350-4F53-ADA8-3A672B89280F}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -974,7 +1307,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F9FDE4-4755-4E32-814A-85CBF4499A47}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -1143,4 +1478,85 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99B01345-7AC3-4EF6-AA31-75067E57E02B}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>80</v>
+      </c>
+      <c r="B2">
+        <v>-1</v>
+      </c>
+      <c r="C2">
+        <v>7.9588781132567599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>90</v>
+      </c>
+      <c r="B3">
+        <v>-1</v>
+      </c>
+      <c r="C3">
+        <v>12.0179667073463</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>-1</v>
+      </c>
+      <c r="C4">
+        <v>17.0552709612701</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>110</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>12.1322115167098</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>120</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>9.02491348345783</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Param1 exact value for K=60
</commit_message>
<xml_diff>
--- a/pyfeng/data/heston_benchmark.xlsx
+++ b/pyfeng/data/heston_benchmark.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PyFENG\pyfeng\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9E0357-D9D3-49F6-AF0E-6062BE3514EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189404E1-1C0F-4F77-A2A3-7CD2E85338AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="743" xr2:uid="{CFD8C97F-677E-4081-BE35-9D7DB797B3CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Param" sheetId="7" r:id="rId1"/>
     <sheet name="1" sheetId="1" r:id="rId2"/>
-    <sheet name="2" sheetId="32" r:id="rId3"/>
-    <sheet name="3" sheetId="31" r:id="rId4"/>
+    <sheet name="2" sheetId="31" r:id="rId3"/>
+    <sheet name="3" sheetId="32" r:id="rId4"/>
     <sheet name="4" sheetId="4" r:id="rId5"/>
     <sheet name="5" sheetId="5" r:id="rId6"/>
     <sheet name="6" sheetId="6" r:id="rId7"/>
@@ -113,15 +113,9 @@
     <t>Tables 2, 5 in Broadie &amp; Kaya (2006), SV-I in Lord et al (2010), Case 5 in Tse &amp; Wan (2013)</t>
   </si>
   <si>
-    <t>Table 2, 3  (Case I) in Van Haastrecht &amp; Pelsser (2010), SV-II in Lord et al (2010), Case 1-3 in Tse &amp; Wan (2013)</t>
-  </si>
-  <si>
     <t>Table 2, 4  (Case II) in Van Haastrecht &amp; Pelsser (2010).</t>
   </si>
   <si>
-    <t>Table 2, 5  (Case III) in Van Haastrecht &amp; Pelsser (2010).</t>
-  </si>
-  <si>
     <t>Figure 6 in Kahl and Jäckel (2005, Wilmott).</t>
   </si>
   <si>
@@ -140,32 +134,31 @@
     <t>divr</t>
   </si>
   <si>
-    <t>https://financepress.com/2019/02/15/heston-model-reference-prices/</t>
-  </si>
-  <si>
     <t>Table A3, Figure 3 (Set I) in von Sydow et al. (2018). BENCHOP - SLV. https://doi.org/10.1080/00207160.2018.1544368</t>
+  </si>
+  <si>
+    <t>Table 2 (Case I) in Andersen (2008), Table 2, 3  (Case I) in Van Haastrecht &amp; Pelsser (2010), SV-II in Lord et al (2010), Case 1-3 in Tse &amp; Wan (2013)</t>
+  </si>
+  <si>
+    <t>Table 3 (Case II) in Andersen (2008), Table 2, 5  (Case III) in Van Haastrecht &amp; Pelsser (2010).</t>
+  </si>
+  <si>
+    <t>Lewis (2019) https://financepress.com/2019/02/15/heston-model-reference-prices/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -194,11 +187,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -207,11 +199,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -524,23 +517,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0584B610-149E-4DFB-B94E-F604CBCB4976}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="6" max="6" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.453125" customWidth="1"/>
+    <col min="7" max="7" width="4.81640625" customWidth="1"/>
     <col min="8" max="8" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.36328125" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -569,13 +566,13 @@
         <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
-        <v>19</v>
-      </c>
-      <c r="L1" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="M1" t="s">
         <v>5</v>
@@ -584,7 +581,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -616,11 +613,11 @@
       <c r="J2" s="5">
         <v>0</v>
       </c>
-      <c r="K2" s="6">
+      <c r="K2" s="9">
         <f>4*C2*F2/(D2*D2)</f>
         <v>0.08</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L2" s="10">
         <f>2*B2*F2*EXP(-F2*G2)/(D2*D2)/(1-EXP(-F2*G2))</f>
         <v>2.7134619625216925E-4</v>
       </c>
@@ -629,110 +626,107 @@
         <v>Price</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.04</v>
+      </c>
+      <c r="C3" s="5">
+        <f t="shared" ref="C3" si="0">B3</f>
+        <v>0.04</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="E3" s="5">
+        <v>-0.5</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.3</v>
+      </c>
+      <c r="G3" s="5">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <f t="shared" ref="A3:A5" si="0">A2+1</f>
-        <v>2</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0.09</v>
-      </c>
-      <c r="C3" s="5">
-        <f>B3</f>
-        <v>0.09</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
-      </c>
-      <c r="E3" s="5">
-        <v>-0.3</v>
-      </c>
-      <c r="F3" s="5">
-        <v>1</v>
-      </c>
-      <c r="G3" s="5">
-        <v>5</v>
-      </c>
       <c r="H3" s="5">
         <v>100</v>
       </c>
       <c r="I3" s="5">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="J3" s="5">
         <v>0</v>
       </c>
-      <c r="K3" s="6">
-        <f t="shared" ref="K3:K10" si="1">4*C3*F3/(D3*D3)</f>
-        <v>0.36</v>
-      </c>
-      <c r="L3" s="5">
-        <f t="shared" ref="L3:L9" si="2">2*B3*F3*EXP(-F3*G3)/(D3*D3)/(1-EXP(-F3*G3))</f>
-        <v>1.2210578831347615E-3</v>
+      <c r="K3" s="9">
+        <f>4*C3*F3/(D3*D3)</f>
+        <v>5.9259259259259255E-2</v>
+      </c>
+      <c r="L3" s="10">
+        <f>2*B3*F3*EXP(-F3*G3)/(D3*D3)/(1-EXP(-F3*G3))</f>
+        <v>3.3285311711068295E-4</v>
       </c>
       <c r="M3" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="M3" ca="1">INDIRECT(A3&amp;"!$B$1")</f>
         <v>Price</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
       <c r="C4" s="5">
-        <f t="shared" ref="C4" si="3">B4</f>
-        <v>0.04</v>
+        <f>B4</f>
+        <v>0.09</v>
       </c>
       <c r="D4" s="5">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E4" s="5">
-        <v>-0.5</v>
+        <v>-0.3</v>
       </c>
       <c r="F4" s="5">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="G4" s="5">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H4" s="5">
         <v>100</v>
       </c>
       <c r="I4" s="5">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J4" s="5">
         <v>0</v>
       </c>
-      <c r="K4" s="6">
-        <f t="shared" si="1"/>
-        <v>5.9259259259259255E-2</v>
-      </c>
-      <c r="L4" s="5">
-        <f t="shared" si="2"/>
-        <v>3.3285311711068295E-4</v>
+      <c r="K4" s="9">
+        <f t="shared" ref="K4:K10" si="1">4*C4*F4/(D4*D4)</f>
+        <v>0.36</v>
+      </c>
+      <c r="L4" s="10">
+        <f t="shared" ref="L4:L9" si="2">2*B4*F4*EXP(-F4*G4)/(D4*D4)/(1-EXP(-F4*G4))</f>
+        <v>1.2210578831347615E-3</v>
       </c>
       <c r="M4" s="3" t="str" cm="1">
         <f t="array" aca="1" ref="M4" ca="1">INDIRECT(A4&amp;"!$B$1")</f>
         <v>Price</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" s="5">
@@ -762,11 +756,11 @@
       <c r="J5" s="5">
         <v>0</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="9">
         <f t="shared" si="1"/>
         <v>1.268368718086536</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="10">
         <f t="shared" si="2"/>
         <v>6.8550309401436851E-4</v>
       </c>
@@ -777,9 +771,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
-        <f t="shared" ref="A6" si="4">A5+1</f>
         <v>5</v>
       </c>
       <c r="B6" s="5">
@@ -809,11 +802,11 @@
       <c r="J6" s="5">
         <v>0</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="9">
         <f t="shared" si="1"/>
         <v>0.72</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="10">
         <f t="shared" si="2"/>
         <v>1.6344716763487597E-5</v>
       </c>
@@ -824,7 +817,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -855,11 +848,11 @@
       <c r="J7" s="5">
         <v>0</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="9">
         <f t="shared" si="1"/>
         <v>0.16</v>
       </c>
-      <c r="L7" s="5">
+      <c r="L7" s="10">
         <f t="shared" si="2"/>
         <v>3.6321592807750218E-6</v>
       </c>
@@ -867,10 +860,10 @@
         <v>11</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -901,11 +894,11 @@
       <c r="J8" s="5">
         <v>0</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="9">
         <f t="shared" si="1"/>
         <v>0.90353478515184005</v>
       </c>
-      <c r="L8" s="5">
+      <c r="L8" s="10">
         <f t="shared" si="2"/>
         <v>2.3645603493803969E-3</v>
       </c>
@@ -916,7 +909,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -947,22 +940,22 @@
       <c r="J9" s="5">
         <v>0.02</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="9">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L9" s="5">
+      <c r="L9" s="10">
         <f t="shared" si="2"/>
         <v>5.9703553164076953E-3</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N9" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -981,7 +974,7 @@
       <c r="F10" s="5">
         <v>4</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="6">
         <v>0.01</v>
       </c>
       <c r="H10" s="5">
@@ -993,22 +986,22 @@
       <c r="J10" s="5">
         <v>0.02</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="9">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="L10" s="5">
-        <f t="shared" ref="L10:L11" si="5">2*B10*F10*EXP(-F10*G10)/(D10*D10)/(1-EXP(-F10*G10))</f>
+      <c r="L10" s="10">
+        <f t="shared" ref="L10:L11" si="3">2*B10*F10*EXP(-F10*G10)/(D10*D10)/(1-EXP(-F10*G10))</f>
         <v>1.9602666595558249</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N10" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N10" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1039,26 +1032,25 @@
       <c r="J11" s="5">
         <v>0</v>
       </c>
-      <c r="K11" s="6">
-        <f t="shared" ref="K11" si="6">4*C11*F11/(D11*D11)</f>
+      <c r="K11" s="9">
+        <f t="shared" ref="K11" si="4">4*C11*F11/(D11*D11)</f>
         <v>0.44375999999999999</v>
       </c>
-      <c r="L11" s="5">
-        <f t="shared" si="5"/>
+      <c r="L11" s="10">
+        <f t="shared" si="3"/>
         <v>4.8227706557066388E-2</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="O11" s="2"/>
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N9" r:id="rId1" xr:uid="{7031F408-D0C8-4303-980A-BE75B855310D}"/>
-    <hyperlink ref="N10" r:id="rId2" xr:uid="{875806D3-0B48-4136-831B-3F4391F03BDC}"/>
+    <hyperlink ref="N9" r:id="rId1" display="https://financepress.com/2019/02/15/heston-model-reference-prices/" xr:uid="{7031F408-D0C8-4303-980A-BE75B855310D}"/>
+    <hyperlink ref="N10" r:id="rId2" display="https://financepress.com/2019/02/15/heston-model-reference-prices/" xr:uid="{875806D3-0B48-4136-831B-3F4391F03BDC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -1077,10 +1069,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
@@ -1151,14 +1143,17 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="12.81640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -1169,7 +1164,7 @@
         <f>100*(100/75)</f>
         <v>133.33333333333331</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="11">
         <f>0.908502728459621*(100/75)</f>
         <v>1.2113369712794946</v>
       </c>
@@ -1178,7 +1173,7 @@
       <c r="A3">
         <v>100</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="11">
         <f>9.04665011922096</f>
         <v>9.0466501192209599</v>
       </c>
@@ -1188,7 +1183,7 @@
         <f>100*(100/125)</f>
         <v>80</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="11">
         <f>28.5147863992987*(100/125)</f>
         <v>22.811829119438961</v>
       </c>
@@ -1201,6 +1196,192 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5761A8C7-5DBE-4514-94EE-A5933B58C928}">
   <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>60</v>
+      </c>
+      <c r="B2" s="4">
+        <v>44.329975070000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>70</v>
+      </c>
+      <c r="B3" s="4">
+        <v>35.849769700000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="4">
+        <v>13.08467014</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>140</v>
+      </c>
+      <c r="B5" s="4">
+        <v>0.29577444000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F9FDE4-4755-4E32-814A-85CBF4499A47}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1">
+        <v>45.286999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3" s="1">
+        <v>16.649000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>140</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5.1379999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FCD568-C350-4F53-ADA8-3A672B89280F}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>60</v>
+      </c>
+      <c r="B2" s="1">
+        <v>56.575000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3" s="1">
+        <v>33.597000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>140</v>
+      </c>
+      <c r="B4" s="1">
+        <v>18.157</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF16E80-6FB9-4334-AC30-EE1DE9F72C5B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" s="4">
+        <v>6.8061133099999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B796A2E3-3674-432B-9CAB-65F8F7D4F037}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1213,189 +1394,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>60</v>
-      </c>
-      <c r="B2" s="4">
-        <v>44.33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>70</v>
-      </c>
-      <c r="B3" s="4">
-        <v>35.849769700000003</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>100</v>
-      </c>
-      <c r="B4" s="4">
-        <v>13.08467014</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>140</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.29577444000000003</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62FCD568-C350-4F53-ADA8-3A672B89280F}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>60</v>
-      </c>
-      <c r="B2" s="1">
-        <v>56.575000000000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>100</v>
-      </c>
-      <c r="B3" s="1">
-        <v>33.597000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>140</v>
-      </c>
-      <c r="B4" s="1">
-        <v>18.157</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0F9FDE4-4755-4E32-814A-85CBF4499A47}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>60</v>
-      </c>
-      <c r="B2" s="1">
-        <v>45.286999999999999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>100</v>
-      </c>
-      <c r="B3" s="1">
-        <v>16.649000000000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>140</v>
-      </c>
-      <c r="B4" s="1">
-        <v>5.1379999999999999</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF16E80-6FB9-4334-AC30-EE1DE9F72C5B}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="10.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>100</v>
-      </c>
-      <c r="B2" s="4">
-        <v>6.8061133099999997</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B796A2E3-3674-432B-9CAB-65F8F7D4F037}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -1418,7 +1417,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4134D2-54E5-4470-946C-B42F18CBD0D8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1427,7 +1428,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -1461,7 +1462,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -1485,17 +1486,17 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
2 more cases added from Ball & Roma (1994)
</commit_message>
<xml_diff>
--- a/pyfeng/data/heston_benchmark.xlsx
+++ b/pyfeng/data/heston_benchmark.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\PyFENG\pyfeng\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{189404E1-1C0F-4F77-A2A3-7CD2E85338AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAB29E2-BE7F-41C7-A568-B4E05631434A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" tabRatio="743" xr2:uid="{CFD8C97F-677E-4081-BE35-9D7DB797B3CD}"/>
   </bookViews>
@@ -24,6 +24,8 @@
     <sheet name="8" sheetId="34" r:id="rId9"/>
     <sheet name="9" sheetId="33" r:id="rId10"/>
     <sheet name="10" sheetId="35" r:id="rId11"/>
+    <sheet name="11" sheetId="36" r:id="rId12"/>
+    <sheet name="12" sheetId="37" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="32">
   <si>
     <t>sigma</t>
   </si>
@@ -144,6 +146,24 @@
   </si>
   <si>
     <t>Lewis (2019) https://financepress.com/2019/02/15/heston-model-reference-prices/</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>OP2</t>
+  </si>
+  <si>
+    <t>OP3</t>
+  </si>
+  <si>
+    <t>Exact</t>
+  </si>
+  <si>
+    <t>Table 1A in Ball &amp; Roma (1994)</t>
+  </si>
+  <si>
+    <t>Table 1B in Ball &amp; Roma (1994)</t>
   </si>
 </sst>
 </file>
@@ -517,13 +537,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0584B610-149E-4DFB-B94E-F604CBCB4976}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -991,7 +1011,7 @@
         <v>4</v>
       </c>
       <c r="L10" s="10">
-        <f t="shared" ref="L10:L11" si="3">2*B10*F10*EXP(-F10*G10)/(D10*D10)/(1-EXP(-F10*G10))</f>
+        <f t="shared" ref="L10:L13" si="3">2*B10*F10*EXP(-F10*G10)/(D10*D10)/(1-EXP(-F10*G10))</f>
         <v>1.9602666595558249</v>
       </c>
       <c r="M10" s="3" t="s">
@@ -1033,7 +1053,7 @@
         <v>0</v>
       </c>
       <c r="K11" s="9">
-        <f t="shared" ref="K11" si="4">4*C11*F11/(D11*D11)</f>
+        <f t="shared" ref="K11:K13" si="4">4*C11*F11/(D11*D11)</f>
         <v>0.44375999999999999</v>
       </c>
       <c r="L11" s="10">
@@ -1045,6 +1065,98 @@
       </c>
       <c r="N11" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.09</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="5">
+        <v>4</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="5">
+        <v>100</v>
+      </c>
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="9">
+        <f t="shared" si="4"/>
+        <v>8.9999999999999982</v>
+      </c>
+      <c r="L12" s="10">
+        <f t="shared" si="3"/>
+        <v>0.70432939237349534</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="5">
+        <v>0.1225</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.1225</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.8</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>8</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="H13" s="5">
+        <v>100</v>
+      </c>
+      <c r="I13" s="5">
+        <v>0</v>
+      </c>
+      <c r="J13" s="5">
+        <v>0</v>
+      </c>
+      <c r="K13" s="9">
+        <f t="shared" si="4"/>
+        <v>6.1249999999999991</v>
+      </c>
+      <c r="L13" s="10">
+        <f t="shared" si="3"/>
+        <v>5.7138166114058003E-2</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1193,6 +1305,243 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E32A6B08-519D-4169-BF8E-2AEB29E981DF}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1">
+        <v>21.425000000000001</v>
+      </c>
+      <c r="C2" s="1">
+        <v>21.43</v>
+      </c>
+      <c r="D2" s="1">
+        <v>21.425999999999998</v>
+      </c>
+      <c r="E2" s="1">
+        <v>21.43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>90</v>
+      </c>
+      <c r="B3" s="1">
+        <v>13.99</v>
+      </c>
+      <c r="C3" s="1">
+        <v>13.933</v>
+      </c>
+      <c r="D3" s="1">
+        <v>13.936999999999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>13.935</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8.4469999999999992</v>
+      </c>
+      <c r="C4" s="1">
+        <v>8.3569999999999993</v>
+      </c>
+      <c r="D4" s="1">
+        <v>8.3670000000000009</v>
+      </c>
+      <c r="E4" s="1">
+        <v>8.359</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>110</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.7460000000000004</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4.6769999999999996</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4.6829999999999998</v>
+      </c>
+      <c r="E5" s="1">
+        <v>4.68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>120</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2.504</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2.4849999999999999</v>
+      </c>
+      <c r="D6" s="1">
+        <v>2.4830000000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>2.4870000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1EED313-9C6E-4407-8CA8-ACB153FA9431}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="8.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1">
+        <v>22.206</v>
+      </c>
+      <c r="C2" s="1">
+        <v>22.19</v>
+      </c>
+      <c r="D2" s="1">
+        <v>22.186</v>
+      </c>
+      <c r="E2" s="1">
+        <v>22.192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>90</v>
+      </c>
+      <c r="B3" s="1">
+        <v>15.186</v>
+      </c>
+      <c r="C3" s="1">
+        <v>15.093999999999999</v>
+      </c>
+      <c r="D3" s="1">
+        <v>15.105</v>
+      </c>
+      <c r="E3" s="1">
+        <v>15.099</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4" s="1">
+        <v>9.8480000000000008</v>
+      </c>
+      <c r="C4" s="1">
+        <v>9.7189999999999994</v>
+      </c>
+      <c r="D4" s="1">
+        <v>9.7379999999999995</v>
+      </c>
+      <c r="E4" s="1">
+        <v>9.7260000000000009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>110</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6.093</v>
+      </c>
+      <c r="C5" s="1">
+        <v>5.9859999999999998</v>
+      </c>
+      <c r="D5" s="1">
+        <v>6</v>
+      </c>
+      <c r="E5" s="1">
+        <v>5.992</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>120</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3.6230000000000002</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3.573</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3.573</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3.5760000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5761A8C7-5DBE-4514-94EE-A5933B58C928}">
   <dimension ref="A1:B5"/>

</xml_diff>